<commit_message>
Adding final layout dynamic tables
</commit_message>
<xml_diff>
--- a/PLANTIILA2.xlsx
+++ b/PLANTIILA2.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uzzie\Documents\Jale\automatizador-crediflexi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A44E271-0E2D-47A8-8770-8D6FFEDCD5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2D0D19-6467-44A1-BC67-AA715D8A41A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="51" r:id="rId6"/>
+    <pivotCache cacheId="23" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8710" uniqueCount="3092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8710" uniqueCount="3093">
   <si>
     <t>Código acreditado</t>
   </si>
@@ -9333,6 +9333,9 @@
   </si>
   <si>
     <t>29/01/1900</t>
+  </si>
+  <si>
+    <t>(blank)</t>
   </si>
 </sst>
 </file>
@@ -9519,7 +9522,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -9583,6 +9586,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -9590,22 +9594,26 @@
     <cellStyle name="Normal 18" xfId="3" xr:uid="{2A504B10-7F54-4E2D-B0E4-83871B6AC25A}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="111">
     <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -9615,21 +9623,93 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -9794,6 +9874,46 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000066"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -9876,46 +9996,6 @@
     </dxf>
     <dxf>
       <alignment vertical="top"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000066"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -10096,8 +10176,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>329205</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>70125</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>127758</xdr:rowOff>
     </xdr:to>
@@ -10197,7 +10277,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Carlos Mejia" refreshedDate="46024.444715625003" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="212" xr:uid="{F1CA2943-AE00-4596-B1C0-C8370C58F79E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Carlos Mejia" refreshedDate="46024.444715625003" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="212" xr:uid="{F1CA2943-AE00-4596-B1C0-C8370C58F79E}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:BQ1048576" sheet="R_Completo"/>
   </cacheSource>
@@ -25513,7 +25593,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D140C8F6-1688-4BFB-94A1-D1EE0E8846FF}" name="TablaDinámica2" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Coordinación">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D140C8F6-1688-4BFB-94A1-D1EE0E8846FF}" name="TablaDinámica2" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Coordinación">
   <location ref="A8:G15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="69">
     <pivotField showAll="0"/>
@@ -25654,10 +25734,10 @@
     <dataField name="Saldo_x000a_Riesgo Total" fld="67" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="20">
-    <format dxfId="90">
+    <format dxfId="105">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="104">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="6">
@@ -25671,10 +25751,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="103">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="87">
+    <format dxfId="102">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="6">
@@ -25688,7 +25768,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="101">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="6">
@@ -25702,14 +25782,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="100">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="99">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -25721,16 +25801,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="98">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="97">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -25739,10 +25819,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="94">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="93">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -25751,7 +25831,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="92">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5" selected="0">
@@ -25764,10 +25844,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="75">
+    <format dxfId="90">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -25776,7 +25856,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="89">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5" selected="0">
@@ -25789,13 +25869,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="88">
       <pivotArea dataOnly="0" grandRow="1" fieldPosition="0"/>
     </format>
-    <format dxfId="72">
+    <format dxfId="87">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="71">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -25812,7 +25892,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CC165D9-9258-4F64-A124-98C3CCC8462F}" name="TablaDinámica3" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="PAR">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CC165D9-9258-4F64-A124-98C3CCC8462F}" name="TablaDinámica3" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="PAR">
   <location ref="J8:S16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="69">
     <pivotField showAll="0"/>
@@ -25970,21 +26050,21 @@
     <dataField name="Suma de Saldo riesgo total" fld="67" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="95">
+    <format dxfId="110">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="14" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="109">
       <pivotArea field="14" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="14" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="108">
       <pivotArea field="14" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="14" count="7" selected="0">
@@ -25999,7 +26079,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="107">
       <pivotArea field="14" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="14" count="7" selected="0">
@@ -26014,7 +26094,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="106">
       <pivotArea field="14" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="14" count="7" selected="0">
@@ -26043,789 +26123,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D799A7A3-4141-4DAD-9761-B8491DE1E75F}" name="TablaDinámica2" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A8:I26" firstHeaderRow="0" firstDataRow="1" firstDataCol="3"/>
-  <pivotFields count="69">
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField name="Coordinación" axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="5"/>
-      </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="8"/>
-      </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="9">
-        <item x="3"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="8"/>
-      </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="2"/>
-    <field x="5"/>
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="18">
-    <i>
-      <x/>
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x v="8"/>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-    <i i="5">
-      <x v="5"/>
-    </i>
-  </colItems>
-  <dataFields count="6">
-    <dataField name="Cantidad_x000a_Prestada" fld="12" baseField="0" baseItem="0"/>
-    <dataField name="Saldo_x000a_Capital" fld="22" baseField="0" baseItem="0"/>
-    <dataField name="Saldo_x000a_Vencido" fld="23" baseField="0" baseItem="0"/>
-    <dataField name="Saldo_x000a_Total" fld="50" baseField="0" baseItem="0"/>
-    <dataField name="Saldo_x000a_Riesgo Capital" fld="66" baseField="0" baseItem="0"/>
-    <dataField name="Saldo_x000a_Riesgo Total" fld="67" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="17">
-    <format dxfId="65">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="64">
-      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="63">
-      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
-    </format>
-    <format dxfId="62">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="6">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="61">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="60">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="5" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="59">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-          <reference field="6" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="58">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="2" count="5" selected="0">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-          </reference>
-          <reference field="5" count="8" selected="0">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-          </reference>
-          <reference field="6" count="8" selected="0">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="57">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="56">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="55">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="54">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="53">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="52">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="51">
-      <pivotArea field="2" grandRow="1" outline="0" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="50">
-      <pivotArea field="2" grandRow="1" outline="0" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="5" selected="0">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="49">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FBEC0F2-77D2-45AE-B5CF-49FDC76AF7B5}" name="TablaDinámica4" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FBEC0F2-77D2-45AE-B5CF-49FDC76AF7B5}" name="TablaDinámica4" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="L7:W26" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="69">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -27473,10 +26771,10 @@
     <dataField name="Suma de Saldo riesgo total" fld="67" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="70">
+    <format dxfId="68">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="69">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="14" count="7">
@@ -27491,7 +26789,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="66">
       <pivotArea field="14" grandRow="1" outline="0" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="14" count="7" selected="0">
@@ -27506,7 +26804,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="65">
       <pivotArea outline="0" fieldPosition="0">
         <references count="4">
           <reference field="2" count="5" selected="0">
@@ -27548,7 +26846,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="64">
       <pivotArea field="14" grandRow="1" outline="0" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="14" count="7" selected="0">
@@ -27576,11 +26874,793 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D799A7A3-4141-4DAD-9761-B8491DE1E75F}" name="TablaDinámica2" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A8:I26" firstHeaderRow="0" firstDataRow="1" firstDataCol="3"/>
+  <pivotFields count="69">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField name="Coordinación" axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="5"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="8"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="9">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="8"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="2"/>
+    <field x="5"/>
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="8"/>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Cantidad_x000a_Prestada" fld="12" baseField="0" baseItem="0"/>
+    <dataField name="Saldo_x000a_Capital" fld="22" baseField="0" baseItem="0"/>
+    <dataField name="Saldo_x000a_Vencido" fld="23" baseField="0" baseItem="0"/>
+    <dataField name="Saldo_x000a_Total" fld="50" baseField="0" baseItem="0"/>
+    <dataField name="Saldo_x000a_Riesgo Capital" fld="66" baseField="0" baseItem="0"/>
+    <dataField name="Saldo_x000a_Riesgo Total" fld="67" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="17">
+    <format dxfId="85">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="84">
+      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="83">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="82">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="6">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="81">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="80">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="79">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+          <reference field="6" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="78">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="2" count="5" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+          <reference field="5" count="8" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+          </reference>
+          <reference field="6" count="8" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="77">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="76">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="75">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="74">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="73">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="72">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="71">
+      <pivotArea field="2" grandRow="1" outline="0" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="70">
+      <pivotArea field="2" grandRow="1" outline="0" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="5" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8EC39BD-4B7F-4A71-B195-8B9EC1F5BAF3}" name="T_181120252" displayName="T_181120252" ref="A2:BQ210">
   <autoFilter ref="A2:BQ210" xr:uid="{B8EC39BD-4B7F-4A71-B195-8B9EC1F5BAF3}"/>
   <tableColumns count="69">
-    <tableColumn id="1" xr3:uid="{F7DB08B5-870E-495A-8398-6C0E1B6B8905}" name="Código acreditado" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{F7DB08B5-870E-495A-8398-6C0E1B6B8905}" name="Código acreditado" dataDxfId="63"/>
     <tableColumn id="2" xr3:uid="{7FD14B16-E62C-4E5E-BD67-BE9E398DEA36}" name="Nom. región"/>
     <tableColumn id="3" xr3:uid="{27653F69-E972-4684-AB44-8276190DC79C}" name="Coordinación"/>
     <tableColumn id="4" xr3:uid="{DAB63D29-BC9D-43A7-9D0E-1C0E06A57D62}" name="Código promotor"/>
@@ -27589,27 +27669,27 @@
     <tableColumn id="7" xr3:uid="{8A85FD84-E1C5-4489-AB30-92254418521D}" name="Nombre recuperador"/>
     <tableColumn id="8" xr3:uid="{634758E6-A850-4E31-A29A-95C8A969C80D}" name="Ciclo"/>
     <tableColumn id="9" xr3:uid="{EFBB40F5-9974-44B3-AD04-ECF14B86BA93}" name="Nombre acreditado"/>
-    <tableColumn id="10" xr3:uid="{A334AD7F-F1B2-4D96-9C0D-BAE0151BE05F}" name="Inicio ciclo" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{8F09DAF2-676E-4E02-9A92-E49174A37CA3}" name="Fin ciclo" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{8695ABD2-41CA-4E24-96AE-98A84BD6AEB6}" name="Cantidad entregada" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{0404A29E-CB5F-416A-8F2A-52B613FCDA6F}" name="Cantidad Prestada" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{A334AD7F-F1B2-4D96-9C0D-BAE0151BE05F}" name="Inicio ciclo" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{8F09DAF2-676E-4E02-9A92-E49174A37CA3}" name="Fin ciclo" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{8695ABD2-41CA-4E24-96AE-98A84BD6AEB6}" name="Cantidad entregada" dataDxfId="60"/>
+    <tableColumn id="13" xr3:uid="{0404A29E-CB5F-416A-8F2A-52B613FCDA6F}" name="Cantidad Prestada" dataDxfId="59"/>
     <tableColumn id="14" xr3:uid="{F6D6CA80-3CB8-435E-81C9-AB2DBCEB2D28}" name="Días de mora"/>
     <tableColumn id="15" xr3:uid="{CC583BAA-748A-4D0E-8E3D-1A14363C2A83}" name="PAR"/>
     <tableColumn id="16" xr3:uid="{984B4A99-BC63-4698-A0B7-F0E6B35BDC01}" name="Plazo del crédito"/>
     <tableColumn id="17" xr3:uid="{E8F8ABFF-EFFD-4E5B-B64A-D58AB9F649E0}" name="Periodicidad"/>
     <tableColumn id="18" xr3:uid="{6D5FEB4C-E7D7-4438-81AE-E327AAFDED47}" name="Parcialidad + Parcialidad comisión"/>
     <tableColumn id="19" xr3:uid="{4BF77CA2-3452-4A11-8A3B-B0F093780DDC}" name="Comisión a pagar"/>
-    <tableColumn id="20" xr3:uid="{507550D1-6A0C-40C2-A501-E81AE6D65011}" name="Interés moratorio saldo vencido total" dataDxfId="43"/>
-    <tableColumn id="21" xr3:uid="{7CB37C1B-BDD0-4B83-B37D-8DBA7BD4B22D}" name="Pagos vencidos" dataDxfId="42"/>
+    <tableColumn id="20" xr3:uid="{507550D1-6A0C-40C2-A501-E81AE6D65011}" name="Interés moratorio saldo vencido total" dataDxfId="58"/>
+    <tableColumn id="21" xr3:uid="{7CB37C1B-BDD0-4B83-B37D-8DBA7BD4B22D}" name="Pagos vencidos" dataDxfId="57"/>
     <tableColumn id="22" xr3:uid="{8D05E370-B379-4500-8F59-6AEF16BB04A7}" name="Periodos vencidos"/>
-    <tableColumn id="23" xr3:uid="{55EB17F8-4C1D-4ADF-90B0-6B249A03F271}" name="Saldo capital" dataDxfId="41"/>
-    <tableColumn id="24" xr3:uid="{3AF7D551-A0B7-439F-892E-6365FC6B4EAB}" name="Saldo vencido" dataDxfId="40"/>
-    <tableColumn id="25" xr3:uid="{4980CF2F-A69A-4B79-B9E9-59B48A939E62}" name="Saldo capital vencido" dataDxfId="39"/>
-    <tableColumn id="26" xr3:uid="{2577AA99-E997-4C6D-8505-7F1032D470B9}" name="Saldo interés vencido" dataDxfId="38"/>
-    <tableColumn id="27" xr3:uid="{4521BBD6-66C6-479C-87AC-94D2E660137D}" name="Saldo comisión vencida" dataDxfId="37"/>
-    <tableColumn id="28" xr3:uid="{775D14A7-1F1F-47F7-9262-B4F4E7C907C1}" name="Saldo recargos" dataDxfId="36"/>
-    <tableColumn id="29" xr3:uid="{3FD5E327-67A8-4DE8-913F-91753A84EE74}" name="$ Último pago" dataDxfId="35"/>
-    <tableColumn id="30" xr3:uid="{CD2D9D92-853B-47AA-9D73-67654F40703A}" name="Último pago" dataDxfId="34"/>
+    <tableColumn id="23" xr3:uid="{55EB17F8-4C1D-4ADF-90B0-6B249A03F271}" name="Saldo capital" dataDxfId="56"/>
+    <tableColumn id="24" xr3:uid="{3AF7D551-A0B7-439F-892E-6365FC6B4EAB}" name="Saldo vencido" dataDxfId="55"/>
+    <tableColumn id="25" xr3:uid="{4980CF2F-A69A-4B79-B9E9-59B48A939E62}" name="Saldo capital vencido" dataDxfId="54"/>
+    <tableColumn id="26" xr3:uid="{2577AA99-E997-4C6D-8505-7F1032D470B9}" name="Saldo interés vencido" dataDxfId="53"/>
+    <tableColumn id="27" xr3:uid="{4521BBD6-66C6-479C-87AC-94D2E660137D}" name="Saldo comisión vencida" dataDxfId="52"/>
+    <tableColumn id="28" xr3:uid="{775D14A7-1F1F-47F7-9262-B4F4E7C907C1}" name="Saldo recargos" dataDxfId="51"/>
+    <tableColumn id="29" xr3:uid="{3FD5E327-67A8-4DE8-913F-91753A84EE74}" name="$ Último pago" dataDxfId="50"/>
+    <tableColumn id="30" xr3:uid="{CD2D9D92-853B-47AA-9D73-67654F40703A}" name="Último pago" dataDxfId="49"/>
     <tableColumn id="31" xr3:uid="{2D1A2F37-1790-485D-8F88-6E158EB5514A}" name="Situación crédito"/>
     <tableColumn id="32" xr3:uid="{5E5D861A-2795-4C75-B7A7-A170EE2850BC}" name="Medio comunic. 1"/>
     <tableColumn id="33" xr3:uid="{E26AD156-4C4D-422D-BE6B-30970552920D}" name="Medio comunic. 2"/>
@@ -27630,8 +27710,8 @@
     <tableColumn id="48" xr3:uid="{6E38C7E3-4741-43C0-880B-108979BAF1D4}" name="Tipo Garantía 2"/>
     <tableColumn id="49" xr3:uid="{6DAC1A55-631F-4C46-A02F-0D741D32DB7A}" name="Descripción garantía 2"/>
     <tableColumn id="50" xr3:uid="{549C1B2A-9802-47C4-ADB0-5BF0B7CCCB64}" name="Garantía 2"/>
-    <tableColumn id="51" xr3:uid="{62127943-EABB-4EC1-9A58-C9A0934B7DC5}" name="Saldo total" dataDxfId="33"/>
-    <tableColumn id="52" xr3:uid="{F66805A6-2583-4DE0-B559-52E74E29EAFF}" name="Saldo adelantado" dataDxfId="32"/>
+    <tableColumn id="51" xr3:uid="{62127943-EABB-4EC1-9A58-C9A0934B7DC5}" name="Saldo total" dataDxfId="48"/>
+    <tableColumn id="52" xr3:uid="{F66805A6-2583-4DE0-B559-52E74E29EAFF}" name="Saldo adelantado" dataDxfId="47"/>
     <tableColumn id="53" xr3:uid="{3F44CAF6-DEA7-4A63-9ACF-CD6A96B3E856}" name="Cód. producto crédito"/>
     <tableColumn id="54" xr3:uid="{95F30154-AF8F-4625-9983-F250FB3F7925}" name="Nom. producto crédito"/>
     <tableColumn id="55" xr3:uid="{0047E5B3-83DE-42EA-ACC7-8078AFBD00DB}" name="Calle"/>
@@ -27639,16 +27719,16 @@
     <tableColumn id="57" xr3:uid="{83950C61-348D-4C63-8147-4AAC2CFC1322}" name="Entidad federativa"/>
     <tableColumn id="58" xr3:uid="{2542A143-5CAE-4091-9D5C-69C2651B6B1E}" name="Municipio"/>
     <tableColumn id="59" xr3:uid="{D92003F6-AAA7-4782-8432-F6D00AC14AC2}" name="Geolocalización domicilio"/>
-    <tableColumn id="60" xr3:uid="{CF8FBBE3-32A2-4F6F-9FD7-13D0D867B201}" name="Link de Geolocalización" dataDxfId="31"/>
+    <tableColumn id="60" xr3:uid="{CF8FBBE3-32A2-4F6F-9FD7-13D0D867B201}" name="Link de Geolocalización" dataDxfId="46"/>
     <tableColumn id="61" xr3:uid="{C17C7A43-0B2F-4AC1-8D52-0D4C13D38EFE}" name="Castigado cartera"/>
     <tableColumn id="62" xr3:uid="{8F678D9E-307E-4ED0-8458-4525D6990D90}" name="Nom. personal castiga cartera"/>
     <tableColumn id="63" xr3:uid="{7352EDEA-B6E9-439A-9CE5-3E215155722C}" name="Frecuencia"/>
     <tableColumn id="64" xr3:uid="{91744B41-C0D4-4732-BDED-7D6319C178C7}" name="Criticidad"/>
     <tableColumn id="65" xr3:uid="{8B37992C-9C2F-43CC-94DD-BB0C2F3A2489}" name="Forma de entrega"/>
-    <tableColumn id="66" xr3:uid="{39763E3B-13A0-4DE2-8AFA-27AA5DF94131}" name="Concepto Depósito" dataDxfId="30"/>
-    <tableColumn id="67" xr3:uid="{B80B3F03-23D9-4025-824D-F1CFBA9C8688}" name="Saldo riesgo capital" dataDxfId="29"/>
-    <tableColumn id="68" xr3:uid="{B8E1CA16-35B0-4189-B6A2-3A7C34F3BB19}" name="Saldo riesgo total" dataDxfId="28"/>
-    <tableColumn id="69" xr3:uid="{0E740140-D86A-436C-9B2A-1745CCB84439}" name="% MORA" dataDxfId="27"/>
+    <tableColumn id="66" xr3:uid="{39763E3B-13A0-4DE2-8AFA-27AA5DF94131}" name="Concepto Depósito" dataDxfId="45"/>
+    <tableColumn id="67" xr3:uid="{B80B3F03-23D9-4025-824D-F1CFBA9C8688}" name="Saldo riesgo capital" dataDxfId="44"/>
+    <tableColumn id="68" xr3:uid="{B8E1CA16-35B0-4189-B6A2-3A7C34F3BB19}" name="Saldo riesgo total" dataDxfId="43"/>
+    <tableColumn id="69" xr3:uid="{0E740140-D86A-436C-9B2A-1745CCB84439}" name="% MORA" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -27658,7 +27738,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{10D46106-5C47-441D-8121-C3F027B37D77}" name="T_18112025" displayName="T_18112025" ref="A2:BQ3" insertRow="1">
   <autoFilter ref="A2:BQ3" xr:uid="{10D46106-5C47-441D-8121-C3F027B37D77}"/>
   <tableColumns count="69">
-    <tableColumn id="1" xr3:uid="{45AB632D-1122-4B80-B84C-B27DAB2FC8B5}" name="Código acreditado" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{45AB632D-1122-4B80-B84C-B27DAB2FC8B5}" name="Código acreditado" dataDxfId="41"/>
     <tableColumn id="2" xr3:uid="{56A60274-305A-4AC1-8E51-953967DA1E68}" name="Nom. región"/>
     <tableColumn id="3" xr3:uid="{BD97A124-225D-40D5-B3E6-985115D7D666}" name="Coordinación"/>
     <tableColumn id="4" xr3:uid="{18C8E859-BA54-491C-B0C9-A8C3932FBDE1}" name="Código promotor"/>
@@ -27667,27 +27747,27 @@
     <tableColumn id="7" xr3:uid="{8E589B69-B8A7-4E98-A83A-6E00296230DD}" name="Nombre recuperador"/>
     <tableColumn id="8" xr3:uid="{B4F1CF15-FD07-4E79-AFFC-CDAA81FE2738}" name="Ciclo"/>
     <tableColumn id="9" xr3:uid="{082FAA69-DBFF-46FC-A7D2-B5E4DDC7E8B7}" name="Nombre acreditado"/>
-    <tableColumn id="10" xr3:uid="{F131CC65-61B3-4ED5-95A6-95F505E9E842}" name="Inicio ciclo" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{34F112EA-0BC7-4EEF-8E28-C0732D18D81A}" name="Fin ciclo" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{4B3AD626-CA83-45D8-83C4-5D7AD6ACA557}" name="Cantidad entregada" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{3883B301-4ED6-4929-86A9-661C41FC3B32}" name="Cantidad Prestada" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{F131CC65-61B3-4ED5-95A6-95F505E9E842}" name="Inicio ciclo" dataDxfId="40"/>
+    <tableColumn id="11" xr3:uid="{34F112EA-0BC7-4EEF-8E28-C0732D18D81A}" name="Fin ciclo" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{4B3AD626-CA83-45D8-83C4-5D7AD6ACA557}" name="Cantidad entregada" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{3883B301-4ED6-4929-86A9-661C41FC3B32}" name="Cantidad Prestada" dataDxfId="37"/>
     <tableColumn id="14" xr3:uid="{AA93B381-3BDA-427B-8EDF-E6354650575C}" name="Días de mora"/>
     <tableColumn id="15" xr3:uid="{800B2624-AB8E-4909-9EE2-4DA7BF5A0A37}" name="PAR"/>
     <tableColumn id="16" xr3:uid="{7A254042-BB5B-4F41-A9D3-DAFAD1D133A2}" name="Plazo del crédito"/>
     <tableColumn id="17" xr3:uid="{9A83C30A-F209-4F6F-B948-5F5AFCC18810}" name="Periodicidad"/>
     <tableColumn id="18" xr3:uid="{083F4FCF-0EDE-4262-AA37-98740F581D76}" name="Parcialidad + Parcialidad comisión"/>
     <tableColumn id="19" xr3:uid="{895E2C82-81B3-4949-AC9D-ACD09DF1FDF6}" name="Comisión a pagar"/>
-    <tableColumn id="20" xr3:uid="{AABC9F03-56A9-40DA-94EC-3F3B267566CC}" name="Interés moratorio saldo vencido total" dataDxfId="21"/>
-    <tableColumn id="21" xr3:uid="{328236F2-7148-4CB9-8512-0D2EDF1BD035}" name="Pagos vencidos" dataDxfId="20"/>
+    <tableColumn id="20" xr3:uid="{AABC9F03-56A9-40DA-94EC-3F3B267566CC}" name="Interés moratorio saldo vencido total" dataDxfId="36"/>
+    <tableColumn id="21" xr3:uid="{328236F2-7148-4CB9-8512-0D2EDF1BD035}" name="Pagos vencidos" dataDxfId="35"/>
     <tableColumn id="22" xr3:uid="{801E3434-C094-4269-9345-72A8C0AE5F55}" name="Periodos vencidos"/>
-    <tableColumn id="23" xr3:uid="{84A22AA9-9BC6-4A39-8EE3-F1400FE2BCA7}" name="Saldo capital" dataDxfId="19"/>
-    <tableColumn id="24" xr3:uid="{2D23D163-4883-4DBD-9994-16C25DAC69B3}" name="Saldo vencido" dataDxfId="18"/>
-    <tableColumn id="25" xr3:uid="{79B1C402-CE9E-487F-9A8E-81311838658B}" name="Saldo capital vencido" dataDxfId="17"/>
-    <tableColumn id="26" xr3:uid="{87F24D6D-B8DC-407A-A2BD-601DB3D425FA}" name="Saldo interés vencido" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{F87BD36D-98E5-4F0E-AEC5-EB267105899F}" name="Saldo comisión vencida" dataDxfId="15"/>
-    <tableColumn id="28" xr3:uid="{93249545-B07B-4A09-808F-9ED828048AC8}" name="Saldo recargos" dataDxfId="14"/>
-    <tableColumn id="29" xr3:uid="{2832DD59-AF7A-4147-A7DC-F3CC07589229}" name="$ Último pago" dataDxfId="13"/>
-    <tableColumn id="30" xr3:uid="{12F63B83-B909-4491-B9C1-2CEA2480DE1A}" name="Último pago" dataDxfId="12"/>
+    <tableColumn id="23" xr3:uid="{84A22AA9-9BC6-4A39-8EE3-F1400FE2BCA7}" name="Saldo capital" dataDxfId="34"/>
+    <tableColumn id="24" xr3:uid="{2D23D163-4883-4DBD-9994-16C25DAC69B3}" name="Saldo vencido" dataDxfId="33"/>
+    <tableColumn id="25" xr3:uid="{79B1C402-CE9E-487F-9A8E-81311838658B}" name="Saldo capital vencido" dataDxfId="32"/>
+    <tableColumn id="26" xr3:uid="{87F24D6D-B8DC-407A-A2BD-601DB3D425FA}" name="Saldo interés vencido" dataDxfId="31"/>
+    <tableColumn id="27" xr3:uid="{F87BD36D-98E5-4F0E-AEC5-EB267105899F}" name="Saldo comisión vencida" dataDxfId="30"/>
+    <tableColumn id="28" xr3:uid="{93249545-B07B-4A09-808F-9ED828048AC8}" name="Saldo recargos" dataDxfId="29"/>
+    <tableColumn id="29" xr3:uid="{2832DD59-AF7A-4147-A7DC-F3CC07589229}" name="$ Último pago" dataDxfId="28"/>
+    <tableColumn id="30" xr3:uid="{12F63B83-B909-4491-B9C1-2CEA2480DE1A}" name="Último pago" dataDxfId="27"/>
     <tableColumn id="31" xr3:uid="{36DC10E2-231A-4BFC-8AB7-ED12061E3D69}" name="Situación crédito"/>
     <tableColumn id="32" xr3:uid="{B89C2B40-4052-49F0-96FB-84B40E829ED8}" name="Medio comunic. 1"/>
     <tableColumn id="33" xr3:uid="{DD12DD5D-3C97-44E0-86DB-8C20C7CFDD1E}" name="Medio comunic. 2"/>
@@ -27708,8 +27788,8 @@
     <tableColumn id="48" xr3:uid="{3DFD0FA7-753D-47E2-9C9F-1B9F89D6A76B}" name="Tipo Garantía 2"/>
     <tableColumn id="49" xr3:uid="{BDEB7300-71A5-4C60-9F66-49D144BECE18}" name="Descripción garantía 2"/>
     <tableColumn id="50" xr3:uid="{5F4A9E4E-9219-4942-9BA8-B91326BB2814}" name="Garantía 2"/>
-    <tableColumn id="51" xr3:uid="{F644ED04-B57A-4F37-B2AB-0732D59FA4A1}" name="Saldo total" dataDxfId="11"/>
-    <tableColumn id="52" xr3:uid="{C8299F8C-588E-47E1-8238-6D88C20505E7}" name="Saldo adelantado" dataDxfId="10"/>
+    <tableColumn id="51" xr3:uid="{F644ED04-B57A-4F37-B2AB-0732D59FA4A1}" name="Saldo total" dataDxfId="26"/>
+    <tableColumn id="52" xr3:uid="{C8299F8C-588E-47E1-8238-6D88C20505E7}" name="Saldo adelantado" dataDxfId="25"/>
     <tableColumn id="53" xr3:uid="{C0B0BA4E-44B2-4020-AE8B-9D18EC27A2E0}" name="Cód. producto crédito"/>
     <tableColumn id="54" xr3:uid="{EB888286-D588-4D37-AE08-EC6A1DA12B16}" name="Nom. producto crédito"/>
     <tableColumn id="55" xr3:uid="{D8E9758C-EFD4-4C30-B8D4-28BA0FAFF4D9}" name="Calle"/>
@@ -27717,16 +27797,16 @@
     <tableColumn id="57" xr3:uid="{913A1172-AA94-4182-89D0-0926C1F936C2}" name="Entidad federativa"/>
     <tableColumn id="58" xr3:uid="{5168D7AF-9E44-4709-AF32-9236572B7471}" name="Municipio"/>
     <tableColumn id="59" xr3:uid="{A38D81F5-CDFB-41B3-B85F-1C19D335B9C4}" name="Geolocalización domicilio"/>
-    <tableColumn id="60" xr3:uid="{A6BDD858-5EA5-4F8C-BA19-7E141A37BA7B}" name="Link de Geolocalización" dataDxfId="9"/>
+    <tableColumn id="60" xr3:uid="{A6BDD858-5EA5-4F8C-BA19-7E141A37BA7B}" name="Link de Geolocalización" dataDxfId="24"/>
     <tableColumn id="61" xr3:uid="{D92129B5-11F2-4C49-8B99-DC60C4E5C841}" name="Castigado cartera"/>
     <tableColumn id="62" xr3:uid="{47F56B99-6911-4E25-A7B4-7E801630D507}" name="Nom. personal castiga cartera"/>
     <tableColumn id="63" xr3:uid="{865F0885-1DC4-43D3-B04E-9F786EFFF365}" name="Frecuencia"/>
     <tableColumn id="64" xr3:uid="{B4520D4E-F6F0-4B56-876C-350E31D27492}" name="Criticidad"/>
     <tableColumn id="65" xr3:uid="{8C28B571-2D1E-4EC5-820E-6EE2E1C02066}" name="Forma de entrega"/>
-    <tableColumn id="66" xr3:uid="{3E65D14E-0B52-4DA4-86AE-A37DA8EB0E3F}" name="Concepto Depósito" dataDxfId="8"/>
-    <tableColumn id="67" xr3:uid="{18AA5489-C623-4E4B-AC5B-2E9C4890EAE1}" name="Saldo riesgo capital" dataDxfId="7"/>
-    <tableColumn id="68" xr3:uid="{A2186643-E023-4F4C-A8B6-1CDFA6DB3D43}" name="Saldo riesgo total" dataDxfId="6"/>
-    <tableColumn id="69" xr3:uid="{E9C1DDC1-9481-41A0-B2F4-C572741C2188}" name="% MORA" dataDxfId="5"/>
+    <tableColumn id="66" xr3:uid="{3E65D14E-0B52-4DA4-86AE-A37DA8EB0E3F}" name="Concepto Depósito" dataDxfId="23"/>
+    <tableColumn id="67" xr3:uid="{18AA5489-C623-4E4B-AC5B-2E9C4890EAE1}" name="Saldo riesgo capital" dataDxfId="22"/>
+    <tableColumn id="68" xr3:uid="{A2186643-E023-4F4C-A8B6-1CDFA6DB3D43}" name="Saldo riesgo total" dataDxfId="21"/>
+    <tableColumn id="69" xr3:uid="{E9C1DDC1-9481-41A0-B2F4-C572741C2188}" name="% MORA" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -28024,12 +28104,13 @@
       <pane xSplit="1" ySplit="8" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.33203125" customWidth="1"/>
     <col min="9" max="9" width="0.109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="14" hidden="1" customWidth="1"/>
@@ -28051,7 +28132,7 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
     </row>
-    <row r="6" spans="1:19" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
@@ -28108,8 +28189,8 @@
         <v>2721</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="0.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:19" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
         <v>2</v>
       </c>
@@ -28142,7 +28223,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="10.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>536</v>
       </c>
@@ -28418,7 +28499,7 @@
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
-        <v>2720</v>
+        <v>3092</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -28459,25 +28540,25 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="39" t="s">
         <v>2907</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="39">
         <v>4791991.08</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="39">
         <v>3209848.5199999996</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="39">
         <v>1743734.1597391195</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="39">
         <v>4787932.9800000004</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="39">
         <v>1575524.5699999998</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G15" s="39">
         <v>2572867.42</v>
       </c>
       <c r="I15" s="29"/>

</xml_diff>